<commit_message>
test: continue to work on test case covering FAO56 example 35
</commit_message>
<xml_diff>
--- a/test/test_data/tables/FAO56_Example_35.xlsx
+++ b/test/test_data/tables/FAO56_Example_35.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\swb_development\git\swb2\test\test_data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C772506-48E5-428D-979D-6CA6B1011D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9F2867-5632-444B-8392-E8C17C6A8465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{2764BA87-3AF3-4B84-9F9D-3E5B1EAC9989}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>0.92</v>

</xml_diff>

<commit_message>
feat: table values work
</commit_message>
<xml_diff>
--- a/test/test_data/tables/FAO56_Example_35.xlsx
+++ b/test/test_data/tables/FAO56_Example_35.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\swb_development\git\swb2\test\test_data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9F2867-5632-444B-8392-E8C17C6A8465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6F5EB5-A2F2-44DC-8A8C-123FF6E0159F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{2764BA87-3AF3-4B84-9F9D-3E5B1EAC9989}"/>
   </bookViews>
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E2">
         <v>0.92</v>

</xml_diff>

<commit_message>
test: further work on FAO-56 unit tests
</commit_message>
<xml_diff>
--- a/test/test_data/tables/FAO56_Example_35.xlsx
+++ b/test/test_data/tables/FAO56_Example_35.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\swb_development\git\swb2\test\test_data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6F5EB5-A2F2-44DC-8A8C-123FF6E0159F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555AE787-6989-4DBE-84A7-158DDE1C3BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{2764BA87-3AF3-4B84-9F9D-3E5B1EAC9989}"/>
   </bookViews>
@@ -59,6 +59,9 @@
     <t>ex35_kcb</t>
   </si>
   <si>
+    <t>ex35_depletion_start</t>
+  </si>
+  <si>
     <t>ex35_kr</t>
   </si>
   <si>
@@ -72,9 +75,6 @@
   </si>
   <si>
     <t>ex35_depletion_end</t>
-  </si>
-  <si>
-    <t>ex35_depletion_start</t>
   </si>
   <si>
     <t>ex35_mean_evap</t>
@@ -439,7 +439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -470,22 +470,22 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
       <c r="O1" t="s">
         <v>14</v>

</xml_diff>